<commit_message>
update chunks and lines statistics
</commit_message>
<xml_diff>
--- a/3. Bears_and_Bugs.jar_Metrics/Bears_Complexity_30_Avg.xlsx
+++ b/3. Bears_and_Bugs.jar_Metrics/Bears_Complexity_30_Avg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="205">
   <si>
     <t>Bears (analysis done Today 04:34 most recent)</t>
   </si>
@@ -1348,6 +1348,18 @@
   </si>
   <si>
     <t>75 total</t>
+  </si>
+  <si>
+    <t>SC Comm</t>
+  </si>
+  <si>
+    <t>MC Comm</t>
+  </si>
+  <si>
+    <t>SL Comm</t>
+  </si>
+  <si>
+    <t>ML Comm</t>
   </si>
 </sst>
 </file>
@@ -2003,7 +2015,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2089,6 +2101,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2548,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH216"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AE97" sqref="AE97:AE98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -5249,7 +5264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>145</v>
       </c>
@@ -5319,7 +5334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>146</v>
       </c>
@@ -5389,7 +5404,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>147</v>
       </c>
@@ -5459,7 +5474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>148</v>
       </c>
@@ -5529,7 +5544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>149</v>
       </c>
@@ -5599,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>150</v>
       </c>
@@ -5669,7 +5684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>151</v>
       </c>
@@ -5739,7 +5754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>152</v>
       </c>
@@ -5809,7 +5824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:32" ht="29.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="14" t="s">
         <v>153</v>
       </c>
@@ -5891,8 +5906,20 @@
         <v>57</v>
       </c>
       <c r="AB73"/>
-    </row>
-    <row r="74" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC73" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD73" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE73" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF73" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>154</v>
       </c>
@@ -5978,8 +6005,24 @@
         <v>NO</v>
       </c>
       <c r="AB74"/>
-    </row>
-    <row r="75" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC74" s="40" t="str">
+        <f>IF(OR(X74="YES", Y74="YES"), "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="AD74" s="40" t="str">
+        <f>IF(OR(Z74="YES", AA74="YES"), "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="AE74" s="1" t="str">
+        <f>X74</f>
+        <v>NO</v>
+      </c>
+      <c r="AF74" s="40" t="str">
+        <f>IF(OR(Y74="YES", AA74="YES"), "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="75" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>156</v>
       </c>
@@ -6065,8 +6108,24 @@
         <v>YES</v>
       </c>
       <c r="AB75"/>
-    </row>
-    <row r="76" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC75" s="40" t="str">
+        <f t="shared" ref="AC75:AC98" si="9">IF(OR(X75="YES", Y75="YES"), "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="AD75" s="40" t="str">
+        <f t="shared" ref="AD75:AD98" si="10">IF(OR(Z75="YES", AA75="YES"), "YES", "NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="AE75" s="1" t="str">
+        <f t="shared" ref="AE75:AE98" si="11">X75</f>
+        <v>NO</v>
+      </c>
+      <c r="AF75" s="40" t="str">
+        <f t="shared" ref="AF75:AF98" si="12">IF(OR(Y75="YES", AA75="YES"), "YES", "NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>157</v>
       </c>
@@ -6152,8 +6211,24 @@
         <v>YES</v>
       </c>
       <c r="AB76"/>
-    </row>
-    <row r="77" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC76" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD76" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>YES</v>
+      </c>
+      <c r="AE76" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF76" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="77" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>158</v>
       </c>
@@ -6239,8 +6314,24 @@
         <v>NO</v>
       </c>
       <c r="AB77"/>
-    </row>
-    <row r="78" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC77" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD77" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE77" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF77" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>159</v>
       </c>
@@ -6326,8 +6417,24 @@
         <v>YES</v>
       </c>
       <c r="AB78"/>
-    </row>
-    <row r="79" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC78" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD78" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>YES</v>
+      </c>
+      <c r="AE78" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF78" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="79" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>160</v>
       </c>
@@ -6413,8 +6520,24 @@
         <v>NO</v>
       </c>
       <c r="AB79"/>
-    </row>
-    <row r="80" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC79" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD79" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE79" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF79" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>161</v>
       </c>
@@ -6500,8 +6623,24 @@
         <v>NO</v>
       </c>
       <c r="AB80"/>
-    </row>
-    <row r="81" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC80" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD80" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE80" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF80" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="81" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>162</v>
       </c>
@@ -6587,8 +6726,24 @@
         <v>NO</v>
       </c>
       <c r="AB81"/>
-    </row>
-    <row r="82" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC81" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD81" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE81" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF81" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="82" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>163</v>
       </c>
@@ -6674,8 +6829,24 @@
         <v>NO</v>
       </c>
       <c r="AB82"/>
-    </row>
-    <row r="83" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC82" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD82" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE82" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF82" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="83" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>164</v>
       </c>
@@ -6761,8 +6932,24 @@
         <v>NO</v>
       </c>
       <c r="AB83"/>
-    </row>
-    <row r="84" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC83" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD83" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE83" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF83" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="84" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
         <v>165</v>
       </c>
@@ -6848,8 +7035,24 @@
         <v>NO</v>
       </c>
       <c r="AB84"/>
-    </row>
-    <row r="85" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC84" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD84" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE84" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF84" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="85" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>170</v>
       </c>
@@ -6935,8 +7138,24 @@
         <v>NO</v>
       </c>
       <c r="AB85"/>
-    </row>
-    <row r="86" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC85" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD85" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE85" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF85" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="86" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>171</v>
       </c>
@@ -7022,8 +7241,24 @@
         <v>NO</v>
       </c>
       <c r="AB86"/>
-    </row>
-    <row r="87" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC86" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD86" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE86" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF86" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="87" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>172</v>
       </c>
@@ -7109,8 +7344,24 @@
         <v>NO</v>
       </c>
       <c r="AB87"/>
-    </row>
-    <row r="88" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC87" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD87" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE87" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF87" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="88" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>173</v>
       </c>
@@ -7196,8 +7447,24 @@
         <v>NO</v>
       </c>
       <c r="AB88"/>
-    </row>
-    <row r="89" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC88" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD88" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE88" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF88" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
         <v>174</v>
       </c>
@@ -7283,8 +7550,24 @@
         <v>NO</v>
       </c>
       <c r="AB89"/>
-    </row>
-    <row r="90" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC89" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD89" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE89" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF89" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>175</v>
       </c>
@@ -7370,8 +7653,24 @@
         <v>NO</v>
       </c>
       <c r="AB90"/>
-    </row>
-    <row r="91" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC90" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD90" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE90" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF90" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="91" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>176</v>
       </c>
@@ -7457,8 +7756,24 @@
         <v>NO</v>
       </c>
       <c r="AB91"/>
-    </row>
-    <row r="92" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC91" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD91" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE91" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF91" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>177</v>
       </c>
@@ -7544,8 +7859,24 @@
         <v>NO</v>
       </c>
       <c r="AB92"/>
-    </row>
-    <row r="93" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC92" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD92" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE92" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF92" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="93" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>178</v>
       </c>
@@ -7631,8 +7962,24 @@
         <v>NO</v>
       </c>
       <c r="AB93"/>
-    </row>
-    <row r="94" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC93" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD93" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE93" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF93" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="94" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>179</v>
       </c>
@@ -7718,8 +8065,24 @@
         <v>NO</v>
       </c>
       <c r="AB94"/>
-    </row>
-    <row r="95" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC94" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD94" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE94" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF94" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="95" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>180</v>
       </c>
@@ -7805,8 +8168,24 @@
         <v>NO</v>
       </c>
       <c r="AB95"/>
-    </row>
-    <row r="96" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC95" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD95" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE95" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF95" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="96" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>181</v>
       </c>
@@ -7892,8 +8271,24 @@
         <v>NO</v>
       </c>
       <c r="AB96"/>
-    </row>
-    <row r="97" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC96" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD96" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE96" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF96" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="97" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>182</v>
       </c>
@@ -7979,8 +8374,24 @@
         <v>NO</v>
       </c>
       <c r="AB97"/>
-    </row>
-    <row r="98" spans="1:28" ht="15" x14ac:dyDescent="0.35">
+      <c r="AC97" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD97" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE97" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF97" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="98" spans="1:32" ht="15" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>183</v>
       </c>
@@ -8066,8 +8477,24 @@
         <v>NO</v>
       </c>
       <c r="AB98"/>
-    </row>
-    <row r="99" spans="1:28" ht="28.8" x14ac:dyDescent="0.35">
+      <c r="AC98" s="40" t="str">
+        <f t="shared" si="9"/>
+        <v>NO</v>
+      </c>
+      <c r="AD98" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>NO</v>
+      </c>
+      <c r="AE98" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>NO</v>
+      </c>
+      <c r="AF98" s="40" t="str">
+        <f t="shared" si="12"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="99" spans="1:32" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A99" s="13" t="s">
         <v>200</v>
       </c>
@@ -8147,435 +8574,447 @@
         <v>57</v>
       </c>
       <c r="AB99"/>
-    </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AC99" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD99" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE99" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF99" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="100" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B100" s="26">
-        <f t="shared" ref="B100:N100" si="9">SUM(B24:B98)</f>
+        <f t="shared" ref="B100:N100" si="13">SUM(B24:B98)</f>
         <v>148.29</v>
       </c>
       <c r="C100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>5630.680000000003</v>
       </c>
       <c r="D100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>897.35000000000014</v>
       </c>
       <c r="E100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>642.76000000000045</v>
       </c>
       <c r="F100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>662.45999999999992</v>
       </c>
       <c r="G100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>198.14999999999992</v>
       </c>
       <c r="H100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>841.01000000000022</v>
       </c>
       <c r="I100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1559.8000000000011</v>
       </c>
       <c r="J100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3821.9900000000002</v>
       </c>
       <c r="K100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>98.660000000000025</v>
       </c>
       <c r="L100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.7665999999999999</v>
       </c>
       <c r="M100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1592.71</v>
       </c>
       <c r="N100" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>88.519999999999953</v>
       </c>
       <c r="O100" s="10"/>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A101" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B101" s="27">
-        <f t="shared" ref="B101:N101" si="10">AVERAGE(B24:B98)</f>
+        <f t="shared" ref="B101:N101" si="14">AVERAGE(B24:B98)</f>
         <v>1.9771999999999998</v>
       </c>
       <c r="C101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>75.075733333333375</v>
       </c>
       <c r="D101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>11.964666666666668</v>
       </c>
       <c r="E101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8.5701333333333398</v>
       </c>
       <c r="F101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8.8327999999999989</v>
       </c>
       <c r="G101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.641999999999999</v>
       </c>
       <c r="H101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>11.213466666666669</v>
       </c>
       <c r="I101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>20.797333333333349</v>
       </c>
       <c r="J101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>50.95986666666667</v>
       </c>
       <c r="K101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.315466666666667</v>
       </c>
       <c r="L101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>3.6887999999999997E-2</v>
       </c>
       <c r="M101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>21.236133333333335</v>
       </c>
       <c r="N101" s="27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.1802666666666661</v>
       </c>
       <c r="O101" s="10"/>
       <c r="P101" s="32">
-        <f t="shared" ref="P101:V101" si="11">AVERAGE(P49:P73)</f>
+        <f t="shared" ref="P101:V101" si="15">AVERAGE(P49:P73)</f>
         <v>1.56</v>
       </c>
       <c r="Q101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.08</v>
       </c>
       <c r="R101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="S101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>3.44</v>
       </c>
       <c r="T101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2.4</v>
       </c>
       <c r="U101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>7.16</v>
       </c>
       <c r="V101" s="32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>15.32</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B102" s="26">
-        <f t="shared" ref="B102:N102" si="12">MIN(B24:B98)</f>
+        <f t="shared" ref="B102:N102" si="16">MIN(B24:B98)</f>
         <v>1</v>
       </c>
       <c r="C102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>68.5</v>
       </c>
       <c r="D102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>5.33</v>
       </c>
       <c r="E102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4.33</v>
       </c>
       <c r="F102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>4.33</v>
       </c>
       <c r="G102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="H102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>6.67</v>
       </c>
       <c r="I102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>9.67</v>
       </c>
       <c r="J102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>22.35</v>
       </c>
       <c r="K102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N102" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O102" s="10"/>
       <c r="P102" s="32">
-        <f t="shared" ref="P102:V102" si="13">AVERAGE(P74:P98)</f>
+        <f t="shared" ref="P102:V102" si="17">AVERAGE(P74:P98)</f>
         <v>3.24</v>
       </c>
       <c r="Q102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1.08</v>
       </c>
       <c r="R102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2.04</v>
       </c>
       <c r="S102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2.52</v>
       </c>
       <c r="T102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1.44</v>
       </c>
       <c r="U102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>6.72</v>
       </c>
       <c r="V102" s="32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>13.28</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A103" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B103" s="27">
-        <f t="shared" ref="B103:N103" si="14">MAX(B24:B98)</f>
+        <f t="shared" ref="B103:N103" si="18">MAX(B24:B98)</f>
         <v>5.88</v>
       </c>
       <c r="C103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>84.67</v>
       </c>
       <c r="D103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>22.5</v>
       </c>
       <c r="E103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>10.71</v>
       </c>
       <c r="F103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="G103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.63</v>
       </c>
       <c r="H103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12.86</v>
       </c>
       <c r="I103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>44.5</v>
       </c>
       <c r="J103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>67.08</v>
       </c>
       <c r="K103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.14</v>
       </c>
       <c r="L103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.17</v>
       </c>
       <c r="M103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>60.82</v>
       </c>
       <c r="N103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3.38</v>
       </c>
       <c r="O103" s="10"/>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B104" s="26">
-        <f t="shared" ref="B104:N104" si="15">_xlfn.STDEV.S(B24:B98)</f>
+        <f t="shared" ref="B104:N104" si="19">_xlfn.STDEV.S(B24:B98)</f>
         <v>1.5373771627484718</v>
       </c>
       <c r="C104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3.4715158202275407</v>
       </c>
       <c r="D104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3.5336671608406456</v>
       </c>
       <c r="E104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1.9535452826005986</v>
       </c>
       <c r="F104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4.3738332992616096</v>
       </c>
       <c r="G104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.9338701802250241</v>
       </c>
       <c r="H104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1.5012089662536348</v>
       </c>
       <c r="I104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>7.8157717077321971</v>
       </c>
       <c r="J104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>9.4934112989003712</v>
       </c>
       <c r="K104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.93970422795475117</v>
       </c>
       <c r="L104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>3.0302086985481317E-2</v>
       </c>
       <c r="M104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>15.177493017830932</v>
       </c>
       <c r="N104" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.8435542138545169</v>
       </c>
       <c r="O104" s="10"/>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A105" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B105" s="27">
-        <f t="shared" ref="B105:N105" si="16">_xlfn.VAR.S(B24:B98)</f>
+        <f t="shared" ref="B105:N105" si="20">_xlfn.VAR.S(B24:B98)</f>
         <v>2.3635285405405408</v>
       </c>
       <c r="C105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>12.051422090090096</v>
       </c>
       <c r="D105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>12.48680360360359</v>
       </c>
       <c r="E105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>3.8163391711710526</v>
       </c>
       <c r="F105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>19.130417729729693</v>
       </c>
       <c r="G105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.87211351351351907</v>
       </c>
       <c r="H105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>2.2536283603603069</v>
       </c>
       <c r="I105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>61.08628738738706</v>
       </c>
       <c r="J105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>90.124858090089248</v>
       </c>
       <c r="K105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.88304403603603487</v>
       </c>
       <c r="L105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>9.1821647567567628E-4</v>
       </c>
       <c r="M105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>230.35629430630669</v>
       </c>
       <c r="N105" s="27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.71158371171171209</v>
       </c>
       <c r="O105" s="10"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A108" s="36" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="1:28" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:32" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" s="35" t="s">
         <v>185</v>
       </c>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:28" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:32" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A110" s="35" t="s">
         <v>186</v>
       </c>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:28" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:32" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A111" s="35" t="s">
         <v>187</v>
       </c>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:28" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:32" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>188</v>
       </c>
@@ -8730,55 +9169,55 @@
         <v>30</v>
       </c>
       <c r="C133" s="32">
-        <f t="shared" ref="C133:O133" si="17" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Buggy",B$24:B$98)</f>
+        <f t="shared" ref="C133:O133" si="21" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Buggy",B$24:B$98)</f>
         <v>1.9787999999999999</v>
       </c>
       <c r="D133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>75.147599999999969</v>
       </c>
       <c r="E133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>11.982800000000003</v>
       </c>
       <c r="F133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>8.5180000000000042</v>
       </c>
       <c r="G133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>8.8940000000000037</v>
       </c>
       <c r="H133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>2.6236000000000002</v>
       </c>
       <c r="I133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>11.142800000000005</v>
       </c>
       <c r="J133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>20.878000000000007</v>
       </c>
       <c r="K133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>50.677199999999985</v>
       </c>
       <c r="L133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.3263999999999998</v>
       </c>
       <c r="M133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>3.3200000000000014E-2</v>
       </c>
       <c r="N133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>20.53520000000001</v>
       </c>
       <c r="O133" s="32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1.1416000000000002</v>
       </c>
     </row>
@@ -8791,55 +9230,55 @@
         <v>62</v>
       </c>
       <c r="C134" s="32">
-        <f t="shared" ref="C134:O134" si="18" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Manual",B$24:B$98)</f>
+        <f t="shared" ref="C134:O134" si="22" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Manual",B$24:B$98)</f>
         <v>2.0096000000000003</v>
       </c>
       <c r="D134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>75.155599999999964</v>
       </c>
       <c r="E134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>11.986799999999999</v>
       </c>
       <c r="F134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8.5188000000000006</v>
       </c>
       <c r="G134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>8.8552000000000017</v>
       </c>
       <c r="H134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>2.6307999999999998</v>
       </c>
       <c r="I134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>11.150400000000005</v>
       </c>
       <c r="J134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>20.840399999999995</v>
       </c>
       <c r="K134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>50.70239999999999</v>
       </c>
       <c r="L134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.3256000000000001</v>
       </c>
       <c r="M134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>3.3200000000000014E-2</v>
       </c>
       <c r="N134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>20.515200000000007</v>
       </c>
       <c r="O134" s="32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.1400000000000001</v>
       </c>
     </row>
@@ -8852,55 +9291,55 @@
         <v>82</v>
       </c>
       <c r="C135" s="32">
-        <f t="shared" ref="C135:O135" si="19" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Auto",B$24:B$98)</f>
+        <f t="shared" ref="C135:O135" si="23" xml:space="preserve"> AVERAGEIF($A$24:$A$98, "*Auto",B$24:B$98)</f>
         <v>1.9432</v>
       </c>
       <c r="D135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>74.924000000000007</v>
       </c>
       <c r="E135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>11.9244</v>
       </c>
       <c r="F135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>8.6735999999999986</v>
       </c>
       <c r="G135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>8.7492000000000019</v>
       </c>
       <c r="H135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>2.6716000000000002</v>
       </c>
       <c r="I135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>11.347199999999997</v>
       </c>
       <c r="J135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>20.6736</v>
       </c>
       <c r="K135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>51.500000000000007</v>
       </c>
       <c r="L135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>1.2944</v>
       </c>
       <c r="M135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4.4264000000000012E-2</v>
       </c>
       <c r="N135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>22.658000000000001</v>
       </c>
       <c r="O135" s="32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>1.2592000000000003</v>
       </c>
     </row>
@@ -9037,55 +9476,55 @@
         <v>63</v>
       </c>
       <c r="C141" s="21">
-        <f t="shared" ref="C141:O141" si="20">AVERAGEIFS(B$49:B$73, $P$49:$P$73, "=1", $P$74:$P$98, "=1")</f>
+        <f t="shared" ref="C141:O141" si="24">AVERAGEIFS(B$49:B$73, $P$49:$P$73, "=1", $P$74:$P$98, "=1")</f>
         <v>3.9399999999999995</v>
       </c>
       <c r="D141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>73.724999999999994</v>
       </c>
       <c r="E141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>15.6675</v>
       </c>
       <c r="F141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>7.4424999999999999</v>
       </c>
       <c r="G141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>14.1775</v>
       </c>
       <c r="H141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>3.2725</v>
       </c>
       <c r="I141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>10.715</v>
       </c>
       <c r="J141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>29.844999999999999</v>
       </c>
       <c r="K141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>53.25</v>
       </c>
       <c r="L141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.5</v>
       </c>
       <c r="M141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="N141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>7.6025</v>
       </c>
       <c r="O141" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.42249999999999999</v>
       </c>
       <c r="R141" s="1">
@@ -9096,55 +9535,55 @@
         <v>64</v>
       </c>
       <c r="T141" s="21" t="e">
-        <f t="shared" ref="T141:AF141" si="21">AVERAGEIFS(B$49:B$73, $X$74:$X$98, "YES")</f>
+        <f t="shared" ref="T141:AF141" si="25">AVERAGEIFS(B$49:B$73, $X$74:$X$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF141" s="21" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9157,55 +9596,55 @@
         <v>83</v>
       </c>
       <c r="C142" s="21">
-        <f t="shared" ref="C142:O142" si="22">AVERAGEIFS(B$74:B$98, $P$49:$P$73, "=1", $P$74:$P$98, "=1")</f>
+        <f t="shared" ref="C142:O142" si="26">AVERAGEIFS(B$74:B$98, $P$49:$P$73, "=1", $P$74:$P$98, "=1")</f>
         <v>3.585</v>
       </c>
       <c r="D142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>74.007500000000007</v>
       </c>
       <c r="E142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>14.7075</v>
       </c>
       <c r="F142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>7.3624999999999998</v>
       </c>
       <c r="G142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>12.925000000000001</v>
       </c>
       <c r="H142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>3.3075000000000001</v>
       </c>
       <c r="I142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>10.672499999999999</v>
       </c>
       <c r="J142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>27.634999999999998</v>
       </c>
       <c r="K142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>52.015000000000001</v>
       </c>
       <c r="L142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
       <c r="M142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="N142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>7.6025</v>
       </c>
       <c r="O142" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.42249999999999999</v>
       </c>
       <c r="R142" s="1">
@@ -9216,55 +9655,55 @@
         <v>84</v>
       </c>
       <c r="T142" s="21" t="e">
-        <f t="shared" ref="T142:AF142" si="23">AVERAGEIFS(B$74:B$98, $X$74:$X$98, "YES")</f>
+        <f t="shared" ref="T142:AF142" si="27">AVERAGEIFS(B$74:B$98, $X$74:$X$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF142" s="21" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9366,55 +9805,55 @@
         <v>65</v>
       </c>
       <c r="C145" s="21">
-        <f t="shared" ref="C145:O145" si="24">AVERAGEIFS(B$49:B$73, $P$49:$P$73, "&gt;1", $P$74:$P$98, "&gt;1")</f>
+        <f t="shared" ref="C145:O145" si="28">AVERAGEIFS(B$49:B$73, $P$49:$P$73, "&gt;1", $P$74:$P$98, "&gt;1")</f>
         <v>2.57</v>
       </c>
       <c r="D145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>80.36</v>
       </c>
       <c r="E145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>9.7899999999999991</v>
       </c>
       <c r="F145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>5.43</v>
       </c>
       <c r="G145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.43</v>
       </c>
       <c r="H145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3.36</v>
       </c>
       <c r="I145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.7899999999999991</v>
       </c>
       <c r="J145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>18.21</v>
       </c>
       <c r="K145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>36.97</v>
       </c>
       <c r="L145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O145" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R145" s="1">
@@ -9425,55 +9864,55 @@
         <v>66</v>
       </c>
       <c r="T145" s="21" t="e">
-        <f t="shared" ref="T145:AF145" si="25">AVERAGEIFS(B$49:B$73, $Y$74:$Y$98, "YES")</f>
+        <f t="shared" ref="T145:AF145" si="29">AVERAGEIFS(B$49:B$73, $Y$74:$Y$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF145" s="21" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9486,55 +9925,55 @@
         <v>85</v>
       </c>
       <c r="C146" s="21">
-        <f t="shared" ref="C146:O146" si="26">AVERAGEIFS(B$74:B$98, $P$49:$P$73, "&gt;1", $P$74:$P$98, "&gt;1")</f>
+        <f t="shared" ref="C146:O146" si="30">AVERAGEIFS(B$74:B$98, $P$49:$P$73, "&gt;1", $P$74:$P$98, "&gt;1")</f>
         <v>2.52</v>
       </c>
       <c r="D146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>80.17</v>
       </c>
       <c r="E146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>10.0175</v>
       </c>
       <c r="F146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.52</v>
       </c>
       <c r="G146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.27</v>
       </c>
       <c r="H146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3.1150000000000002</v>
       </c>
       <c r="I146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>8.6374999999999993</v>
       </c>
       <c r="J146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>18.287500000000001</v>
       </c>
       <c r="K146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>36.277499999999996</v>
       </c>
       <c r="L146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="M146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O146" s="21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R146" s="1">
@@ -9545,55 +9984,55 @@
         <v>86</v>
       </c>
       <c r="T146" s="21" t="e">
-        <f t="shared" ref="T146:AF146" si="27">AVERAGEIFS(B$74:B$98, $Y$74:$Y$98, "YES")</f>
+        <f t="shared" ref="T146:AF146" si="31">AVERAGEIFS(B$74:B$98, $Y$74:$Y$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF146" s="21" t="e">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9721,55 +10160,55 @@
         <v>67</v>
       </c>
       <c r="C149" s="21" t="e">
-        <f t="shared" ref="C149:O149" si="28">AVERAGEIFS(B$49:B$73, $U$49:$U$73, "=1", $U$74:$U$98, "=1")</f>
+        <f t="shared" ref="C149:O149" si="32">AVERAGEIFS(B$49:B$73, $U$49:$U$73, "=1", $U$74:$U$98, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O149" s="21" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R149" s="1">
@@ -9780,55 +10219,55 @@
         <v>68</v>
       </c>
       <c r="T149" s="21" t="e">
-        <f t="shared" ref="T149:AF149" si="29">AVERAGEIFS(B$49:B$73, $Z$74:$Z$98, "YES")</f>
+        <f t="shared" ref="T149:AF149" si="33">AVERAGEIFS(B$49:B$73, $Z$74:$Z$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF149" s="21" t="e">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9841,55 +10280,55 @@
         <v>87</v>
       </c>
       <c r="C150" s="21" t="e">
-        <f t="shared" ref="C150:O150" si="30">AVERAGEIFS(B$74:B$98, $U$49:$U$73, "=1", $U$74:$U$98, "=1")</f>
+        <f t="shared" ref="C150:O150" si="34">AVERAGEIFS(B$74:B$98, $U$49:$U$73, "=1", $U$74:$U$98, "=1")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O150" s="21" t="e">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R150" s="1">
@@ -9900,55 +10339,55 @@
         <v>88</v>
       </c>
       <c r="T150" s="21" t="e">
-        <f t="shared" ref="T150:AF150" si="31">AVERAGEIFS(B$74:B$98, $Z$74:$Z$98, "YES")</f>
+        <f t="shared" ref="T150:AF150" si="35">AVERAGEIFS(B$74:B$98, $Z$74:$Z$98, "YES")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF150" s="21" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10076,55 +10515,55 @@
         <v>69</v>
       </c>
       <c r="C153" s="21">
-        <f t="shared" ref="C153:O153" si="32">AVERAGEIFS(B$49:B$73, $U$49:$U$73, "&gt;1", $U$74:$U$98, "&gt;1")</f>
+        <f t="shared" ref="C153:O153" si="36">AVERAGEIFS(B$49:B$73, $U$49:$U$73, "&gt;1", $U$74:$U$98, "&gt;1")</f>
         <v>2.57</v>
       </c>
       <c r="D153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>80.36</v>
       </c>
       <c r="E153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9.7899999999999991</v>
       </c>
       <c r="F153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>5.43</v>
       </c>
       <c r="G153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8.43</v>
       </c>
       <c r="H153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.36</v>
       </c>
       <c r="I153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8.7899999999999991</v>
       </c>
       <c r="J153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>18.21</v>
       </c>
       <c r="K153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>36.97</v>
       </c>
       <c r="L153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O153" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="R153" s="1">
@@ -10135,55 +10574,55 @@
         <v>70</v>
       </c>
       <c r="T153" s="21">
-        <f t="shared" ref="T153:AF153" si="33">AVERAGEIFS(B$49:B$73, $AA$74:$AA$98, "YES")</f>
+        <f t="shared" ref="T153:AF153" si="37">AVERAGEIFS(B$49:B$73, $AA$74:$AA$98, "YES")</f>
         <v>2.57</v>
       </c>
       <c r="U153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>80.36</v>
       </c>
       <c r="V153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>9.7899999999999991</v>
       </c>
       <c r="W153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>5.43</v>
       </c>
       <c r="X153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>8.43</v>
       </c>
       <c r="Y153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3.36</v>
       </c>
       <c r="Z153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>8.7899999999999991</v>
       </c>
       <c r="AA153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>18.21</v>
       </c>
       <c r="AB153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>36.97</v>
       </c>
       <c r="AC153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AD153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AE153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="AF153" s="21">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -10196,55 +10635,55 @@
         <v>89</v>
       </c>
       <c r="C154" s="21">
-        <f t="shared" ref="C154:O154" si="34">AVERAGEIFS(B$74:B$98, $U$49:$U$73, "&gt;1", $U$74:$U$98, "&gt;1")</f>
+        <f t="shared" ref="C154:O154" si="38">AVERAGEIFS(B$74:B$98, $U$49:$U$73, "&gt;1", $U$74:$U$98, "&gt;1")</f>
         <v>2.52</v>
       </c>
       <c r="D154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>80.17</v>
       </c>
       <c r="E154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>10.0175</v>
       </c>
       <c r="F154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>5.52</v>
       </c>
       <c r="G154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>8.27</v>
       </c>
       <c r="H154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>3.1150000000000002</v>
       </c>
       <c r="I154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>8.6374999999999993</v>
       </c>
       <c r="J154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>18.287500000000001</v>
       </c>
       <c r="K154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>36.277499999999996</v>
       </c>
       <c r="L154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="M154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O154" s="21">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R154" s="1">
@@ -10255,55 +10694,55 @@
         <v>90</v>
       </c>
       <c r="T154" s="21">
-        <f t="shared" ref="T154:AF154" si="35">AVERAGEIFS(B$74:B$98, $AA$74:$AA$98, "YES")</f>
+        <f t="shared" ref="T154:AF154" si="39">AVERAGEIFS(B$74:B$98, $AA$74:$AA$98, "YES")</f>
         <v>2.5133333333333332</v>
       </c>
       <c r="U154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>80.100000000000009</v>
       </c>
       <c r="V154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>9.9966666666666679</v>
       </c>
       <c r="W154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>5.54</v>
       </c>
       <c r="X154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>8.2333333333333325</v>
       </c>
       <c r="Y154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>3.1033333333333335</v>
       </c>
       <c r="Z154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>8.6433333333333326</v>
       </c>
       <c r="AA154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>18.23</v>
       </c>
       <c r="AB154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>36.206666666666671</v>
       </c>
       <c r="AC154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF154" s="21">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
@@ -10399,55 +10838,55 @@
         <v>49</v>
       </c>
       <c r="C160" s="21">
-        <f t="shared" ref="C160:O160" si="36">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C160:O160" si="40">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Buggy", B$24:B$98)</f>
         <v>4.58</v>
       </c>
       <c r="D160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>72.25</v>
       </c>
       <c r="E160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>16.25</v>
       </c>
       <c r="F160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>6.73</v>
       </c>
       <c r="G160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>15.13</v>
       </c>
       <c r="H160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>4.63</v>
       </c>
       <c r="I160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>11.37</v>
       </c>
       <c r="J160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>31.38</v>
       </c>
       <c r="K160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>56.97</v>
       </c>
       <c r="L160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="M160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="N160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>13.41</v>
       </c>
       <c r="O160" s="21">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0.75</v>
       </c>
     </row>
@@ -10460,55 +10899,55 @@
         <v>71</v>
       </c>
       <c r="C161" s="21">
-        <f t="shared" ref="C161:O161" si="37">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C161:O161" si="41">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Manual", B$24:B$98)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="D161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>72</v>
       </c>
       <c r="E161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>16.420000000000002</v>
       </c>
       <c r="F161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>6.79</v>
       </c>
       <c r="G161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>15.15</v>
       </c>
       <c r="H161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>4.62</v>
       </c>
       <c r="I161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>11.42</v>
       </c>
       <c r="J161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>31.57</v>
       </c>
       <c r="K161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>57.34</v>
       </c>
       <c r="L161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0.56999999999999995</v>
       </c>
       <c r="M161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="N161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>13.16</v>
       </c>
       <c r="O161" s="21">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0.73</v>
       </c>
     </row>
@@ -10521,55 +10960,55 @@
         <v>91</v>
       </c>
       <c r="C162" s="21">
-        <f t="shared" ref="C162:O162" si="38">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C162:O162" si="42">AVERAGEIF($A$24:$A$98, "*albfernandez-GDS-PMD-Security*_Auto", B$24:B$98)</f>
         <v>4.58</v>
       </c>
       <c r="D162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>72.27</v>
       </c>
       <c r="E162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>16.259999999999998</v>
       </c>
       <c r="F162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>6.73</v>
       </c>
       <c r="G162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>15.11</v>
       </c>
       <c r="H162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>4.625</v>
       </c>
       <c r="I162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>11.36</v>
       </c>
       <c r="J162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>31.365000000000002</v>
       </c>
       <c r="K162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>56.94</v>
       </c>
       <c r="L162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0.53</v>
       </c>
       <c r="M162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>1.03E-2</v>
       </c>
       <c r="N162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>12.344999999999999</v>
       </c>
       <c r="O162" s="21">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>0.68500000000000005</v>
       </c>
     </row>
@@ -10626,55 +11065,55 @@
         <v>50</v>
       </c>
       <c r="C165" s="21">
-        <f t="shared" ref="C165:O165" si="39">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C165:O165" si="43">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Buggy", B$24:B$98)</f>
         <v>2.33</v>
       </c>
       <c r="D165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>84.67</v>
       </c>
       <c r="E165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>5.33</v>
       </c>
       <c r="F165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>4.33</v>
       </c>
       <c r="G165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>4.33</v>
       </c>
       <c r="H165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>2.33</v>
       </c>
       <c r="I165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>6.67</v>
       </c>
       <c r="J165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>9.67</v>
       </c>
       <c r="K165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>22.35</v>
       </c>
       <c r="L165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="M165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="N165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="O165" s="21">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
     </row>
@@ -10687,55 +11126,55 @@
         <v>72</v>
       </c>
       <c r="C166" s="21">
-        <f t="shared" ref="C166:O166" si="40">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C166:O166" si="44">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Manual", B$24:B$98)</f>
         <v>3</v>
       </c>
       <c r="D166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>83.33</v>
       </c>
       <c r="E166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>6.67</v>
       </c>
       <c r="F166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>4.67</v>
       </c>
       <c r="G166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>6</v>
       </c>
       <c r="H166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>2.33</v>
       </c>
       <c r="I166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="J166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>12.67</v>
       </c>
       <c r="K166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>26.04</v>
       </c>
       <c r="L166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="M166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="N166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="O166" s="21">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -10748,55 +11187,55 @@
         <v>92</v>
       </c>
       <c r="C167" s="21">
-        <f t="shared" ref="C167:O167" si="41">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C167:O167" si="45">AVERAGEIF($A$24:$A$98, "*dungba88-libra*_Auto", B$24:B$98)</f>
         <v>2.33</v>
       </c>
       <c r="D167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>84.67</v>
       </c>
       <c r="E167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>5.33</v>
       </c>
       <c r="F167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>4.33</v>
       </c>
       <c r="G167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>4.33</v>
       </c>
       <c r="H167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>2.33</v>
       </c>
       <c r="I167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>6.67</v>
       </c>
       <c r="J167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>9.67</v>
       </c>
       <c r="K167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>22.35</v>
       </c>
       <c r="L167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="M167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="N167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O167" s="21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -10853,55 +11292,55 @@
         <v>51</v>
       </c>
       <c r="C170" s="21" t="e">
-        <f t="shared" ref="C170:O170" si="42">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C170:O170" si="46">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Buggy", B$24:B$98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O170" s="21" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10914,55 +11353,55 @@
         <v>73</v>
       </c>
       <c r="C171" s="21" t="e">
-        <f t="shared" ref="C171:O171" si="43">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C171:O171" si="47">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Manual", B$24:B$98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O171" s="21" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10975,55 +11414,55 @@
         <v>93</v>
       </c>
       <c r="C172" s="21" t="e">
-        <f t="shared" ref="C172:O172" si="44">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C172:O172" si="48">AVERAGEIF($A$24:$A$98, "*julianps-modelmapper-module*_Auto", B$24:B$98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O172" s="21" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11080,55 +11519,55 @@
         <v>52</v>
       </c>
       <c r="C175" s="21">
-        <f t="shared" ref="C175:O175" si="45">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C175:O175" si="49">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Buggy", B$24:B$98)</f>
         <v>2.62</v>
       </c>
       <c r="D175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>79.849999999999994</v>
       </c>
       <c r="E175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>10.31</v>
       </c>
       <c r="F175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>5.54</v>
       </c>
       <c r="G175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>8.69</v>
       </c>
       <c r="H175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>3.31</v>
       </c>
       <c r="I175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>8.85</v>
       </c>
       <c r="J175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>19</v>
       </c>
       <c r="K175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>37.72</v>
       </c>
       <c r="L175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="M175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="N175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="O175" s="21">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
     </row>
@@ -11141,55 +11580,55 @@
         <v>74</v>
       </c>
       <c r="C176" s="21">
-        <f t="shared" ref="C176:O176" si="46">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C176:O176" si="50">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Manual", B$24:B$98)</f>
         <v>2.57</v>
       </c>
       <c r="D176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>80.36</v>
       </c>
       <c r="E176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>9.7899999999999991</v>
       </c>
       <c r="F176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>5.43</v>
       </c>
       <c r="G176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>8.43</v>
       </c>
       <c r="H176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>3.36</v>
       </c>
       <c r="I176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>8.7899999999999991</v>
       </c>
       <c r="J176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>18.21</v>
       </c>
       <c r="K176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>36.97</v>
       </c>
       <c r="L176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="M176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="N176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="O176" s="21">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
     </row>
@@ -11202,55 +11641,55 @@
         <v>94</v>
       </c>
       <c r="C177" s="21">
-        <f t="shared" ref="C177:O177" si="47">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C177:O177" si="51">AVERAGEIF($A$24:$A$98, "*opentracing-contrib-java-p6sp*_Auto", B$24:B$98)</f>
         <v>2.52</v>
       </c>
       <c r="D177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>80.17</v>
       </c>
       <c r="E177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>10.0175</v>
       </c>
       <c r="F177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>5.52</v>
       </c>
       <c r="G177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>8.27</v>
       </c>
       <c r="H177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>3.1150000000000002</v>
       </c>
       <c r="I177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>8.6374999999999993</v>
       </c>
       <c r="J177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>18.287500000000001</v>
       </c>
       <c r="K177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>36.277499999999996</v>
       </c>
       <c r="L177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="N177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O177" s="21">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
@@ -11307,55 +11746,55 @@
         <v>53</v>
       </c>
       <c r="C180" s="21">
-        <f t="shared" ref="C180:O180" si="48">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C180:O180" si="52">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Buggy", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>74.569999999999965</v>
       </c>
       <c r="E180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>11</v>
       </c>
       <c r="F180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>9.860000000000003</v>
       </c>
       <c r="G180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>6.86</v>
       </c>
       <c r="H180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="I180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>11.860000000000003</v>
       </c>
       <c r="J180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>17.860000000000007</v>
       </c>
       <c r="K180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>52.87</v>
       </c>
       <c r="L180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="N180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>30.410000000000011</v>
       </c>
       <c r="O180" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>1.6900000000000004</v>
       </c>
     </row>
@@ -11368,55 +11807,55 @@
         <v>75</v>
       </c>
       <c r="C181" s="22">
-        <f t="shared" ref="C181:O181" si="49">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C181:O181" si="53">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Manual", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>74.569999999999965</v>
       </c>
       <c r="E181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>11</v>
       </c>
       <c r="F181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>9.860000000000003</v>
       </c>
       <c r="G181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>6.7099999999999973</v>
       </c>
       <c r="H181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="I181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>11.860000000000003</v>
       </c>
       <c r="J181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>17.710000000000004</v>
       </c>
       <c r="K181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>52.799999999999983</v>
       </c>
       <c r="L181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="M181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="N181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>30.410000000000011</v>
       </c>
       <c r="O181" s="22">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>1.6900000000000004</v>
       </c>
     </row>
@@ -11429,55 +11868,55 @@
         <v>95</v>
       </c>
       <c r="C182" s="22">
-        <f t="shared" ref="C182:O182" si="50">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C182:O182" si="54">AVERAGEIF($A$24:$A$98, "*SzFMV2018-Tavasz-AutomatedCar*_Auto", B$24:B$98)</f>
         <v>1.00875</v>
       </c>
       <c r="D182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>74.106875000000016</v>
       </c>
       <c r="E182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>11.105625</v>
       </c>
       <c r="F182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>10.115624999999998</v>
       </c>
       <c r="G182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>6.9206249999999994</v>
       </c>
       <c r="H182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>2.1243750000000001</v>
       </c>
       <c r="I182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>12.241250000000001</v>
       </c>
       <c r="J182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>18.026250000000001</v>
       </c>
       <c r="K182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>54.658124999999998</v>
       </c>
       <c r="L182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>1.9562499999999998</v>
       </c>
       <c r="M182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>6.7875000000000019E-2</v>
       </c>
       <c r="N182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>33.860000000000007</v>
       </c>
       <c r="O182" s="22">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>1.8818750000000004</v>
       </c>
     </row>
@@ -11534,55 +11973,55 @@
         <v>54</v>
       </c>
       <c r="C185" s="21">
-        <f t="shared" ref="C185:O185" si="51">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Buggy", B$24:B$98)</f>
+        <f t="shared" ref="C185:O185" si="55">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Buggy", B$24:B$98)</f>
         <v>5.75</v>
       </c>
       <c r="D185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>68.5</v>
       </c>
       <c r="E185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>22.25</v>
       </c>
       <c r="F185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>7.62</v>
       </c>
       <c r="G185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>21.62</v>
       </c>
       <c r="H185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>4.38</v>
       </c>
       <c r="I185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>12</v>
       </c>
       <c r="J185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>43.88</v>
       </c>
       <c r="K185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>66.92</v>
       </c>
       <c r="L185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="M185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="N185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="O185" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
     </row>
@@ -11595,55 +12034,55 @@
         <v>76</v>
       </c>
       <c r="C186" s="22">
-        <f t="shared" ref="C186:O186" si="52">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Manual", B$24:B$98)</f>
+        <f t="shared" ref="C186:O186" si="56">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Manual", B$24:B$98)</f>
         <v>5.88</v>
       </c>
       <c r="D186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>68.5</v>
       </c>
       <c r="E186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>22.5</v>
       </c>
       <c r="F186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>7.62</v>
       </c>
       <c r="G186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>22</v>
       </c>
       <c r="H186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>4.38</v>
       </c>
       <c r="I186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>12</v>
       </c>
       <c r="J186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>44.5</v>
       </c>
       <c r="K186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>67.08</v>
       </c>
       <c r="L186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="M186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="N186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="O186" s="22">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
     </row>
@@ -11656,55 +12095,55 @@
         <v>96</v>
       </c>
       <c r="C187" s="22">
-        <f t="shared" ref="C187:O187" si="53">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Auto", B$24:B$98)</f>
+        <f t="shared" ref="C187:O187" si="57">AVERAGEIF($A$24:$A$98, "*traccar-traccar*_Auto", B$24:B$98)</f>
         <v>5.4350000000000005</v>
       </c>
       <c r="D187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>68.75</v>
       </c>
       <c r="E187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>21.25</v>
       </c>
       <c r="F187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>7.5600000000000005</v>
       </c>
       <c r="G187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>20.185000000000002</v>
       </c>
       <c r="H187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>4.38</v>
       </c>
       <c r="I187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>11.940000000000001</v>
       </c>
       <c r="J187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>41.435000000000002</v>
       </c>
       <c r="K187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>65.814999999999998</v>
       </c>
       <c r="L187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="M187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="N187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="O187" s="22">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
     </row>
@@ -11800,55 +12239,55 @@
         <v>77</v>
       </c>
       <c r="C193" s="21">
-        <f t="shared" ref="C193:O193" si="54">AVERAGEIF($A$24:$A$98, "Arja*Manual", B$24:B$98)</f>
+        <f t="shared" ref="C193:O193" si="58">AVERAGEIF($A$24:$A$98, "Arja*Manual", B$24:B$98)</f>
         <v>2.3418181818181818</v>
       </c>
       <c r="D193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>75.89</v>
       </c>
       <c r="E193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>12.098181818181816</v>
       </c>
       <c r="F193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>7.7663636363636357</v>
       </c>
       <c r="G193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>9.4927272727272722</v>
       </c>
       <c r="H193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>2.9490909090909088</v>
       </c>
       <c r="I193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>10.716363636363637</v>
       </c>
       <c r="J193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>21.587272727272733</v>
       </c>
       <c r="K193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>48.754545454545458</v>
       </c>
       <c r="L193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.96090909090909093</v>
       </c>
       <c r="M193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>2.4090909090909093E-2</v>
       </c>
       <c r="N193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>15.019090909090909</v>
       </c>
       <c r="O193" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.83454545454545437</v>
       </c>
     </row>
@@ -11861,55 +12300,55 @@
         <v>97</v>
       </c>
       <c r="C194" s="25">
-        <f t="shared" ref="C194:O194" si="55">AVERAGEIF($A$24:$A$98, "Arja*Auto", B$24:B$98)</f>
+        <f t="shared" ref="C194:O194" si="59">AVERAGEIF($A$24:$A$98, "Arja*Auto", B$24:B$98)</f>
         <v>2.2645454545454546</v>
       </c>
       <c r="D194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>75.788181818181812</v>
       </c>
       <c r="E194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>11.982727272727272</v>
       </c>
       <c r="F194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>7.8209090909090913</v>
       </c>
       <c r="G194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>9.3072727272727285</v>
       </c>
       <c r="H194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>2.9</v>
       </c>
       <c r="I194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>10.722727272727271</v>
       </c>
       <c r="J194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>21.29</v>
       </c>
       <c r="K194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>48.667272727272731</v>
       </c>
       <c r="L194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0.98272727272727256</v>
       </c>
       <c r="M194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>2.7E-2</v>
       </c>
       <c r="N194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>17.775454545454547</v>
       </c>
       <c r="O194" s="25">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0.98818181818181816</v>
       </c>
     </row>
@@ -11922,55 +12361,55 @@
         <v>78</v>
       </c>
       <c r="C195" s="21">
-        <f t="shared" ref="C195:O195" si="56">AVERAGEIF($A$24:$A$98, "GenProg*Manual", B$24:B$98)</f>
+        <f t="shared" ref="C195:O195" si="60">AVERAGEIF($A$24:$A$98, "GenProg*Manual", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>74.569999999999993</v>
       </c>
       <c r="E195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>11</v>
       </c>
       <c r="F195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>9.86</v>
       </c>
       <c r="G195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>6.7099999999999991</v>
       </c>
       <c r="H195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>2</v>
       </c>
       <c r="I195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>11.86</v>
       </c>
       <c r="J195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>17.71</v>
       </c>
       <c r="K195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>52.8</v>
       </c>
       <c r="L195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>2</v>
       </c>
       <c r="M195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>0.05</v>
       </c>
       <c r="N195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>30.410000000000004</v>
       </c>
       <c r="O195" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>1.69</v>
       </c>
     </row>
@@ -11983,55 +12422,55 @@
         <v>98</v>
       </c>
       <c r="C196" s="25">
-        <f t="shared" ref="C196:O196" si="57">AVERAGEIF($A$24:$A$98, "GenProg*Auto", B$24:B$98)</f>
+        <f t="shared" ref="C196:O196" si="61">AVERAGEIF($A$24:$A$98, "GenProg*Auto", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>73.486000000000004</v>
       </c>
       <c r="E196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>11.2</v>
       </c>
       <c r="F196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>10.370000000000001</v>
       </c>
       <c r="G196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>7.202</v>
       </c>
       <c r="H196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>2.2280000000000002</v>
       </c>
       <c r="I196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>12.6</v>
       </c>
       <c r="J196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>18.398000000000003</v>
       </c>
       <c r="K196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>56.54</v>
       </c>
       <c r="L196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>1.9440000000000002</v>
       </c>
       <c r="M196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="N196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>36.606000000000002</v>
       </c>
       <c r="O196" s="25">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>2.0339999999999998</v>
       </c>
     </row>
@@ -12044,55 +12483,55 @@
         <v>79</v>
       </c>
       <c r="C197" s="21">
-        <f t="shared" ref="C197:O197" si="58">AVERAGEIF($A$24:$A$98, "Kali*Manual", B$24:B$98)</f>
+        <f t="shared" ref="C197:O197" si="62">AVERAGEIF($A$24:$A$98, "Kali*Manual", B$24:B$98)</f>
         <v>3.62</v>
       </c>
       <c r="D197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>74.599999999999994</v>
       </c>
       <c r="E197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>14.147500000000001</v>
       </c>
       <c r="F197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>7.2350000000000003</v>
       </c>
       <c r="G197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>12.465</v>
       </c>
       <c r="H197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>3.3324999999999996</v>
       </c>
       <c r="I197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>10.57</v>
       </c>
       <c r="J197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>26.612500000000001</v>
       </c>
       <c r="K197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>50.814999999999998</v>
       </c>
       <c r="L197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>0.64249999999999996</v>
       </c>
       <c r="M197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>1.6250000000000001E-2</v>
       </c>
       <c r="N197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>10.8925</v>
       </c>
       <c r="O197" s="21">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>0.60499999999999998</v>
       </c>
     </row>
@@ -12105,55 +12544,55 @@
         <v>99</v>
       </c>
       <c r="C198" s="25">
-        <f t="shared" ref="C198:O198" si="59">AVERAGEIF($A$24:$A$98, "Kali*Auto", B$24:B$98)</f>
+        <f t="shared" ref="C198:O198" si="63">AVERAGEIF($A$24:$A$98, "Kali*Auto", B$24:B$98)</f>
         <v>3.4175000000000004</v>
       </c>
       <c r="D198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>74.825000000000003</v>
       </c>
       <c r="E198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>13.65</v>
       </c>
       <c r="F198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>7.1700000000000008</v>
       </c>
       <c r="G198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>11.8</v>
       </c>
       <c r="H198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>3.3674999999999997</v>
       </c>
       <c r="I198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>10.54</v>
       </c>
       <c r="J198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>25.45</v>
       </c>
       <c r="K198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>49.992500000000007</v>
       </c>
       <c r="L198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>0.63500000000000001</v>
       </c>
       <c r="M198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>1.3900000000000001E-2</v>
       </c>
       <c r="N198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>10.807500000000001</v>
       </c>
       <c r="O198" s="25">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>0.6</v>
       </c>
     </row>
@@ -12166,55 +12605,55 @@
         <v>80</v>
       </c>
       <c r="C199" s="21" t="e">
-        <f t="shared" ref="C199:O199" si="60">AVERAGEIF($A$24:$A$98, "Nopol*Manual", B$24:B$98)</f>
+        <f t="shared" ref="C199:O199" si="64">AVERAGEIF($A$24:$A$98, "Nopol*Manual", B$24:B$98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O199" s="21" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -12227,55 +12666,55 @@
         <v>100</v>
       </c>
       <c r="C200" s="25" t="e">
-        <f t="shared" ref="C200:O200" si="61">AVERAGEIF($A$24:$A$98, "Nopol*Auto", B$24:B$98)</f>
+        <f t="shared" ref="C200:O200" si="65">AVERAGEIF($A$24:$A$98, "Nopol*Auto", B$24:B$98)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O200" s="25" t="e">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -12288,55 +12727,55 @@
         <v>81</v>
       </c>
       <c r="C201" s="21">
-        <f t="shared" ref="C201:O201" si="62">AVERAGEIF($A$24:$A$98, "RSRepair*Manual", B$24:B$98)</f>
+        <f t="shared" ref="C201:O201" si="66">AVERAGEIF($A$24:$A$98, "RSRepair*Manual", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>74.569999999999993</v>
       </c>
       <c r="E201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>11</v>
       </c>
       <c r="F201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>9.86</v>
       </c>
       <c r="G201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>6.7099999999999991</v>
       </c>
       <c r="H201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>2</v>
       </c>
       <c r="I201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>11.86</v>
       </c>
       <c r="J201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>17.71</v>
       </c>
       <c r="K201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>52.8</v>
       </c>
       <c r="L201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>2</v>
       </c>
       <c r="M201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>0.05</v>
       </c>
       <c r="N201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>30.410000000000004</v>
       </c>
       <c r="O201" s="21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>1.69</v>
       </c>
     </row>
@@ -12349,55 +12788,55 @@
         <v>101</v>
       </c>
       <c r="C202" s="25">
-        <f t="shared" ref="C202:O202" si="63">AVERAGEIF($A$24:$A$98, "RSRepair*Auto", B$24:B$98)</f>
+        <f t="shared" ref="C202:O202" si="67">AVERAGEIF($A$24:$A$98, "RSRepair*Auto", B$24:B$98)</f>
         <v>1</v>
       </c>
       <c r="D202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>74.539999999999992</v>
       </c>
       <c r="E202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>11.14</v>
       </c>
       <c r="F202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>10.056000000000001</v>
       </c>
       <c r="G202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>6.6280000000000001</v>
       </c>
       <c r="H202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.056</v>
       </c>
       <c r="I202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>12.114000000000001</v>
       </c>
       <c r="J202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>17.772000000000002</v>
       </c>
       <c r="K202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>53.898000000000003</v>
       </c>
       <c r="L202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.8579999999999999</v>
       </c>
       <c r="M202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>5.28E-2</v>
       </c>
       <c r="N202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>28.931999999999999</v>
       </c>
       <c r="O202" s="25">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>1.6079999999999999</v>
       </c>
     </row>

</xml_diff>